<commit_message>
intial ensembles 2-6 added
</commit_message>
<xml_diff>
--- a/Advocacy/drawdown calcs.xlsx
+++ b/Advocacy/drawdown calcs.xlsx
@@ -1,23 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davem\Documents\GWModel\Aguaseca_Project\Advocacy\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CD91AE-212B-4AE4-9386-E549D7F0225C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="24526"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10530" yWindow="3220" windowWidth="8690" windowHeight="6000" xr2:uid="{EF00B51A-2BF7-4D96-861A-988504B6FEEA}"/>
+    <workbookView xWindow="10120" yWindow="920" windowWidth="16900" windowHeight="12780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -69,8 +65,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +92,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -150,6 +151,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,7 +212,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -262,7 +264,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -456,32 +458,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB304EDD-E74B-477F-BEED-12B82081505B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="15" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="38" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -511,7 +513,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="15" thickBot="1">
       <c r="A3" s="1">
         <v>1333113</v>
       </c>
@@ -522,7 +524,7 @@
         <v>-4.3899999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="15" thickBot="1">
       <c r="A4" s="1">
         <v>3133113</v>
       </c>
@@ -533,48 +535,62 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="18" thickBot="1">
       <c r="A5" s="1">
         <v>3111331</v>
       </c>
       <c r="B5" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C5" s="6">
+        <v>-0.57617189999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" thickBot="1">
       <c r="A6" s="1">
         <v>1111331</v>
       </c>
       <c r="B6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C6" s="3">
+        <v>-9.8889999999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1">
       <c r="A7" s="1">
         <v>2121331</v>
       </c>
       <c r="B7" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C7">
+        <v>-2.137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1">
       <c r="A8" s="1">
         <v>2121311</v>
       </c>
       <c r="B8" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C8">
+        <v>-2.1480000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1">
       <c r="A9" s="1">
         <v>2122111</v>
       </c>
       <c r="B9" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C9">
+        <v>-2.1480000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1">
       <c r="A10" s="1">
         <v>2213223</v>
       </c>
@@ -585,7 +601,7 @@
         <v>-0.99639999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" ht="15" thickBot="1">
       <c r="A11" s="1">
         <v>2211221</v>
       </c>
@@ -596,7 +612,7 @@
         <v>-1.383</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" ht="15" thickBot="1">
       <c r="A12" s="1">
         <v>1111111</v>
       </c>
@@ -614,25 +630,30 @@
         <v>2.7484463641257553</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10">
       <c r="B13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10">
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10">
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:2">
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2">
       <c r="B18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added increased pumping(x1.25) for intial baseline
</commit_message>
<xml_diff>
--- a/Advocacy/drawdown calcs.xlsx
+++ b/Advocacy/drawdown calcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10120" yWindow="920" windowWidth="16900" windowHeight="12780"/>
+    <workbookView xWindow="5780" yWindow="0" windowWidth="19680" windowHeight="13520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Advocacy</t>
   </si>
@@ -60,13 +60,19 @@
   </si>
   <si>
     <t>Average:</t>
+  </si>
+  <si>
+    <t>more pump drawdown</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +103,22 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Courier New"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,8 +153,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -153,7 +177,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -466,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -641,11 +667,190 @@
     <row r="16" spans="1:10">
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="1:5" ht="15" thickBot="1">
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="2:2">
-      <c r="B18" s="3"/>
+    <row r="18" spans="1:5" ht="38" thickBot="1">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" thickBot="1">
+      <c r="A19" s="1">
+        <v>1333113</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4">
+        <v>-4.3899999999999997</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" thickBot="1">
+      <c r="A20" s="1">
+        <v>3133113</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18" thickBot="1">
+      <c r="A21" s="1">
+        <v>3111331</v>
+      </c>
+      <c r="B21" s="5">
+        <v>2</v>
+      </c>
+      <c r="C21" s="6">
+        <v>-0.57617189999999996</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickBot="1">
+      <c r="A22" s="1">
+        <v>1111331</v>
+      </c>
+      <c r="B22" s="5">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3">
+        <v>-9.8889999999999993</v>
+      </c>
+      <c r="D22">
+        <v>-10.02</v>
+      </c>
+      <c r="E22">
+        <f>(1-(C22/D22))*100</f>
+        <v>1.307385229540925</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" thickBot="1">
+      <c r="A23" s="1">
+        <v>2121331</v>
+      </c>
+      <c r="B23" s="5">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>-2.137</v>
+      </c>
+      <c r="D23">
+        <v>-2.19</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ref="E23:E28" si="0">(1-(C23/D23))*100</f>
+        <v>2.4200913242009126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" thickBot="1">
+      <c r="A24" s="1">
+        <v>2121311</v>
+      </c>
+      <c r="B24" s="5">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>-2.1480000000000001</v>
+      </c>
+      <c r="D24">
+        <v>-2.21</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>2.8054298642533837</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" thickBot="1">
+      <c r="A25" s="1">
+        <v>2122111</v>
+      </c>
+      <c r="B25" s="5">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>-2.1480000000000001</v>
+      </c>
+      <c r="D25">
+        <v>-2.21</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>2.8054298642533837</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" thickBot="1">
+      <c r="A26" s="1">
+        <v>2213223</v>
+      </c>
+      <c r="B26" s="5">
+        <v>7</v>
+      </c>
+      <c r="C26" s="3">
+        <v>-0.99639999999999995</v>
+      </c>
+      <c r="D26">
+        <v>-1.0149999999999999</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>1.8325123152709288</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" thickBot="1">
+      <c r="A27" s="1">
+        <v>2211221</v>
+      </c>
+      <c r="B27" s="5">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>-1.383</v>
+      </c>
+      <c r="D27">
+        <v>-1.44</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>3.9583333333333304</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" thickBot="1">
+      <c r="A28" s="1">
+        <v>1111111</v>
+      </c>
+      <c r="B28" s="5">
+        <v>9</v>
+      </c>
+      <c r="C28" s="3">
+        <v>-10.046112000000001</v>
+      </c>
+      <c r="D28">
+        <v>-10.210000000000001</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>1.6051714005876572</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
more pumping well moved added
</commit_message>
<xml_diff>
--- a/Advocacy/drawdown calcs.xlsx
+++ b/Advocacy/drawdown calcs.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Advocacy</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>more pump well moved</t>
+  </si>
+  <si>
+    <t>percent change</t>
   </si>
 </sst>
 </file>
@@ -484,7 +490,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -494,14 +500,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1">
@@ -667,84 +673,79 @@
     <row r="16" spans="1:10">
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1">
+    <row r="17" spans="1:9" ht="15" thickBot="1">
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:5" ht="38" thickBot="1">
+    <row r="18" spans="1:9" ht="15" thickBot="1">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>3</v>
+      <c r="C18" t="s">
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" thickBot="1">
       <c r="A19" s="1">
         <v>1333113</v>
       </c>
       <c r="B19" s="5">
         <v>0</v>
       </c>
-      <c r="C19" s="4">
-        <v>-4.3899999999999997</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1">
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" thickBot="1">
       <c r="A20" s="1">
         <v>3133113</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
       </c>
-      <c r="C20" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="18" thickBot="1">
+    <row r="21" spans="1:9" ht="15" thickBot="1">
       <c r="A21" s="1">
         <v>3111331</v>
       </c>
       <c r="B21" s="5">
         <v>2</v>
       </c>
-      <c r="C21" s="6">
-        <v>-0.57617189999999996</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1">
+    <row r="22" spans="1:9" ht="18" thickBot="1">
       <c r="A22" s="1">
         <v>1111331</v>
       </c>
       <c r="B22" s="5">
         <v>3</v>
       </c>
-      <c r="C22" s="3">
-        <v>-9.8889999999999993</v>
+      <c r="C22">
+        <v>-10.02</v>
       </c>
       <c r="D22">
-        <v>-10.02</v>
+        <v>-9.76</v>
       </c>
       <c r="E22">
-        <f>(1-(C22/D22))*100</f>
-        <v>1.307385229540925</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1">
+        <f>(1-D22/C22)*100</f>
+        <v>2.5948103792415189</v>
+      </c>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="1:9" ht="18" thickBot="1">
       <c r="A23" s="1">
         <v>2121331</v>
       </c>
@@ -752,17 +753,18 @@
         <v>4</v>
       </c>
       <c r="C23">
-        <v>-2.137</v>
+        <v>-2.19</v>
       </c>
       <c r="D23">
-        <v>-2.19</v>
+        <v>-2.13</v>
       </c>
       <c r="E23">
-        <f t="shared" ref="E23:E28" si="0">(1-(C23/D23))*100</f>
-        <v>2.4200913242009126</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15" thickBot="1">
+        <f>(1-D23/C23)*100</f>
+        <v>2.7397260273972601</v>
+      </c>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="1:9" ht="18" thickBot="1">
       <c r="A24" s="1">
         <v>2121311</v>
       </c>
@@ -770,17 +772,18 @@
         <v>5</v>
       </c>
       <c r="C24">
-        <v>-2.1480000000000001</v>
+        <v>-2.21</v>
       </c>
       <c r="D24">
-        <v>-2.21</v>
+        <v>-2.15</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
-        <v>2.8054298642533837</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1">
+        <f>(1-D24/C24)*100</f>
+        <v>2.714932126696834</v>
+      </c>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="1:9" ht="18" thickBot="1">
       <c r="A25" s="1">
         <v>2122111</v>
       </c>
@@ -788,35 +791,37 @@
         <v>6</v>
       </c>
       <c r="C25">
-        <v>-2.1480000000000001</v>
+        <v>-2.21</v>
       </c>
       <c r="D25">
-        <v>-2.21</v>
+        <v>-2.15</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
-        <v>2.8054298642533837</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1">
+        <f>(1-D25/C25)*100</f>
+        <v>2.714932126696834</v>
+      </c>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:9" ht="18" thickBot="1">
       <c r="A26" s="1">
         <v>2213223</v>
       </c>
       <c r="B26" s="5">
         <v>7</v>
       </c>
-      <c r="C26" s="3">
-        <v>-0.99639999999999995</v>
+      <c r="C26">
+        <v>-1.0149999999999999</v>
       </c>
       <c r="D26">
-        <v>-1.0149999999999999</v>
+        <v>-0.92</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
-        <v>1.8325123152709288</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1">
+        <f>(1-D26/C26)*100</f>
+        <v>9.3596059113300374</v>
+      </c>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:9" ht="18" thickBot="1">
       <c r="A27" s="1">
         <v>2211221</v>
       </c>
@@ -824,33 +829,35 @@
         <v>8</v>
       </c>
       <c r="C27">
-        <v>-1.383</v>
+        <v>-1.44</v>
       </c>
       <c r="D27">
-        <v>-1.44</v>
+        <v>-1.37</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
-        <v>3.9583333333333304</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1">
+        <f>(1-D27/C27)*100</f>
+        <v>4.8611111111111054</v>
+      </c>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="1:9" ht="18" thickBot="1">
       <c r="A28" s="1">
         <v>1111111</v>
       </c>
       <c r="B28" s="5">
         <v>9</v>
       </c>
-      <c r="C28" s="3">
-        <v>-10.046112000000001</v>
+      <c r="C28">
+        <v>-10.210000000000001</v>
       </c>
       <c r="D28">
-        <v>-10.210000000000001</v>
+        <v>-10</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
-        <v>1.6051714005876572</v>
-      </c>
+        <f>(1-D28/C28)*100</f>
+        <v>2.0568070519099035</v>
+      </c>
+      <c r="I28" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
a bunch of runs
</commit_message>
<xml_diff>
--- a/Advocacy/drawdown calcs.xlsx
+++ b/Advocacy/drawdown calcs.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="24526"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachelspinti/Documents/HWRS_582/Aguaseca_Project/Advocacy/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D627EBBA-2110-8645-859E-9AD1E49CF002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5780" yWindow="0" windowWidth="19680" windowHeight="13520"/>
+    <workbookView xWindow="1100" yWindow="460" windowWidth="27820" windowHeight="19020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -25,6 +28,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -77,8 +83,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +115,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Courier New"/>
+      <family val="1"/>
     </font>
     <font>
       <u/>
@@ -125,6 +132,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF303F9F"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,7 +183,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -175,13 +194,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -490,32 +514,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:14" ht="16" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="38" thickBot="1">
+    <row r="2" spans="1:14" ht="45" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -544,139 +568,286 @@
         <v>5</v>
       </c>
       <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" ht="20" thickBot="1">
       <c r="A3" s="1">
         <v>1333113</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>0</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="6">
         <v>-4.3899999999999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="6">
+        <v>-4.3836975000000002</v>
+      </c>
+      <c r="G3" s="7">
+        <f>ABS(((F3-C3)/F3)*100)</f>
+        <v>0.14377132546211122</v>
+      </c>
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4" spans="1:14" ht="20" thickBot="1">
       <c r="A4" s="1">
         <v>3133113</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="6">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="18" thickBot="1">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="6">
+        <v>-0.48382567999999998</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:G12" si="0">ABS(((F4-C4)/F4)*100)</f>
+        <v>3.3430056875029908</v>
+      </c>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:14" ht="20" thickBot="1">
       <c r="A5" s="1">
         <v>3111331</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>2</v>
       </c>
       <c r="C5" s="6">
         <v>-0.57617189999999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1">
+      <c r="D5">
+        <v>-0.53250120000000001</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" ref="E5:E11" si="1">(C5-D5) /C5 * 100</f>
+        <v>7.5794567558744115</v>
+      </c>
+      <c r="F5" s="7">
+        <v>-0.56997679999999995</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0869038880179001</v>
+      </c>
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="1:14" ht="20" thickBot="1">
       <c r="A6" s="1">
         <v>1111331</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>3</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="6">
         <v>-9.8889999999999993</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+      <c r="D6">
+        <v>-9.6519659999999998</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="1"/>
+        <v>2.3969461017291893</v>
+      </c>
+      <c r="F6" s="7">
+        <v>-9.765053</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2692916259645426</v>
+      </c>
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="1:14" ht="20" thickBot="1">
       <c r="A7" s="1">
         <v>2121331</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>4</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="7">
         <v>-2.137</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1">
+      <c r="D7">
+        <v>-2.0276565999999998</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="1"/>
+        <v>5.1166775854001028</v>
+      </c>
+      <c r="F7" s="7">
+        <v>-2.1143339999999999</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0720160580116516</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="1:14" ht="20" thickBot="1">
       <c r="A8" s="1">
         <v>2121311</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>5</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="7">
         <v>-2.1480000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+      <c r="D8">
+        <v>-2.0350646999999999</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="1"/>
+        <v>5.2576955307262656</v>
+      </c>
+      <c r="F8" s="7">
+        <v>-2.1297760000000001</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" si="0"/>
+        <v>0.85567684113258946</v>
+      </c>
+      <c r="K8" s="8"/>
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" ht="20" thickBot="1">
       <c r="A9" s="1">
         <v>2122111</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>6</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="7">
         <v>-2.1480000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1">
+      <c r="D9">
+        <v>-2.0354766999999998</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="1"/>
+        <v>5.238514897579158</v>
+      </c>
+      <c r="F9" s="7">
+        <v>-2.1286315999999998</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" si="0"/>
+        <v>0.90989911077145935</v>
+      </c>
+      <c r="K9" s="8"/>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="1:14" ht="20" thickBot="1">
       <c r="A10" s="1">
         <v>2213223</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>7</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="6">
         <v>-0.99639999999999995</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1">
+      <c r="D10">
+        <v>-0.96211239999999998</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="1"/>
+        <v>3.4411481332798046</v>
+      </c>
+      <c r="F10" s="7">
+        <v>-0.95437620000000001</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" si="0"/>
+        <v>4.4032740967345942</v>
+      </c>
+      <c r="K10" s="8"/>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:14" ht="20" thickBot="1">
       <c r="A11" s="1">
         <v>2211221</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>8</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="7">
         <v>-1.383</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1">
+      <c r="D11">
+        <v>-1.2331467</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="1"/>
+        <v>10.835379609544466</v>
+      </c>
+      <c r="F11" s="7">
+        <v>-1.3412476</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="0"/>
+        <v>3.1129524481534969</v>
+      </c>
+      <c r="K11" s="8"/>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:14" ht="20" thickBot="1">
       <c r="A12" s="1">
         <v>1111111</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>9</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="6">
         <v>-10.046112000000001</v>
       </c>
       <c r="D12">
-        <v>-9.77</v>
-      </c>
-      <c r="E12">
+        <v>-9.7687840000000001</v>
+      </c>
+      <c r="E12" s="7">
         <f>(C12-D12) /C12 * 100</f>
-        <v>2.7484463641257553</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>2.7605505493070419</v>
+      </c>
+      <c r="F12" s="7">
+        <v>-9.9868509999999997</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.59339024883820857</v>
+      </c>
+      <c r="K12" s="8"/>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:14">
       <c r="B13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="1:14">
       <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="1:14" ht="19">
       <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1">
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" ht="16" thickBot="1">
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="15" thickBot="1">
+    <row r="18" spans="1:9" ht="16" thickBot="1">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -690,11 +861,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1">
+    <row r="19" spans="1:9" ht="16" thickBot="1">
       <c r="A19" s="1">
         <v>1333113</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>0</v>
       </c>
       <c r="C19" t="s">
@@ -704,33 +875,33 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1">
+    <row r="20" spans="1:9" ht="16" thickBot="1">
       <c r="A20" s="1">
         <v>3133113</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>1</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1">
+    <row r="21" spans="1:9" ht="16" thickBot="1">
       <c r="A21" s="1">
         <v>3111331</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <v>2</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="18" thickBot="1">
+    <row r="22" spans="1:9" ht="20" thickBot="1">
       <c r="A22" s="1">
         <v>1111331</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>3</v>
       </c>
       <c r="C22">
@@ -740,16 +911,16 @@
         <v>-9.76</v>
       </c>
       <c r="E22">
-        <f>(1-D22/C22)*100</f>
+        <f t="shared" ref="E22:E28" si="2">(1-D22/C22)*100</f>
         <v>2.5948103792415189</v>
       </c>
-      <c r="I22" s="6"/>
-    </row>
-    <row r="23" spans="1:9" ht="18" thickBot="1">
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" ht="20" thickBot="1">
       <c r="A23" s="1">
         <v>2121331</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <v>4</v>
       </c>
       <c r="C23">
@@ -759,16 +930,16 @@
         <v>-2.13</v>
       </c>
       <c r="E23">
-        <f>(1-D23/C23)*100</f>
+        <f t="shared" si="2"/>
         <v>2.7397260273972601</v>
       </c>
-      <c r="I23" s="6"/>
-    </row>
-    <row r="24" spans="1:9" ht="18" thickBot="1">
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" ht="20" thickBot="1">
       <c r="A24" s="1">
         <v>2121311</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <v>5</v>
       </c>
       <c r="C24">
@@ -778,16 +949,16 @@
         <v>-2.15</v>
       </c>
       <c r="E24">
-        <f>(1-D24/C24)*100</f>
+        <f t="shared" si="2"/>
         <v>2.714932126696834</v>
       </c>
-      <c r="I24" s="6"/>
-    </row>
-    <row r="25" spans="1:9" ht="18" thickBot="1">
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:9" ht="20" thickBot="1">
       <c r="A25" s="1">
         <v>2122111</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>6</v>
       </c>
       <c r="C25">
@@ -797,16 +968,16 @@
         <v>-2.15</v>
       </c>
       <c r="E25">
-        <f>(1-D25/C25)*100</f>
+        <f t="shared" si="2"/>
         <v>2.714932126696834</v>
       </c>
-      <c r="I25" s="6"/>
-    </row>
-    <row r="26" spans="1:9" ht="18" thickBot="1">
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" ht="16" thickBot="1">
       <c r="A26" s="1">
         <v>2213223</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <v>7</v>
       </c>
       <c r="C26">
@@ -816,16 +987,15 @@
         <v>-0.92</v>
       </c>
       <c r="E26">
-        <f>(1-D26/C26)*100</f>
+        <f t="shared" si="2"/>
         <v>9.3596059113300374</v>
       </c>
-      <c r="I26" s="6"/>
-    </row>
-    <row r="27" spans="1:9" ht="18" thickBot="1">
+    </row>
+    <row r="27" spans="1:9" ht="16" thickBot="1">
       <c r="A27" s="1">
         <v>2211221</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="4">
         <v>8</v>
       </c>
       <c r="C27">
@@ -835,16 +1005,15 @@
         <v>-1.37</v>
       </c>
       <c r="E27">
-        <f>(1-D27/C27)*100</f>
+        <f t="shared" si="2"/>
         <v>4.8611111111111054</v>
       </c>
-      <c r="I27" s="6"/>
-    </row>
-    <row r="28" spans="1:9" ht="18" thickBot="1">
+    </row>
+    <row r="28" spans="1:9" ht="16" thickBot="1">
       <c r="A28" s="1">
         <v>1111111</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="4">
         <v>9</v>
       </c>
       <c r="C28">
@@ -854,10 +1023,9 @@
         <v>-10</v>
       </c>
       <c r="E28">
-        <f>(1-D28/C28)*100</f>
+        <f t="shared" si="2"/>
         <v>2.0568070519099035</v>
       </c>
-      <c r="I28" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>